<commit_message>
Added spatial and csv data to map
converted spatial to geojson and added to map; joined to csv attribute data
</commit_message>
<xml_diff>
--- a/data/restaurant_cdc_data.xlsx
+++ b/data/restaurant_cdc_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheri\Documents\geog575\d3-coordinated-viz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46310D68-5D63-4F31-B6C4-7A37F371480D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29698AB3-D516-4A97-BFE9-CF9857C6FF5C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9327F420-2EC5-4128-BAD2-205FBE22B46D}"/>
+    <workbookView xWindow="396" yWindow="0" windowWidth="12012" windowHeight="12120" xr2:uid="{9327F420-2EC5-4128-BAD2-205FBE22B46D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
     <t>state_name</t>
   </si>
   <si>
-    <t>state_abb</t>
+    <t>STUSPS</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>